<commit_message>
Complete VTOL hover roll control.
</commit_message>
<xml_diff>
--- a/parameters/controlParameters.xlsx
+++ b/parameters/controlParameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomo\TomoCode\aae451\aae451-senior-design\parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9013B8CF-DEEA-4A35-9CAF-230576DD99A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F58601D-29D3-4504-9FD5-15B717D04C53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28020" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Forward (Cold) Post xdist</t>
   </si>
@@ -33,12 +33,6 @@
     <t>Aft (Hot )Post xdist</t>
   </si>
   <si>
-    <t>Forward (Cold) Post ydist</t>
-  </si>
-  <si>
-    <t>Aft (Hot )Post ydist</t>
-  </si>
-  <si>
     <t>Engine Centerpoint ydist</t>
   </si>
   <si>
@@ -46,6 +40,18 @@
   </si>
   <si>
     <t>MaxThrust</t>
+  </si>
+  <si>
+    <t>Forward (Cold) Post ydist far</t>
+  </si>
+  <si>
+    <t>Aft (Hot )Post ydist far</t>
+  </si>
+  <si>
+    <t>Forward (Cold) Post ydist close</t>
+  </si>
+  <si>
+    <t>Aft (Hot )Post ydist close</t>
   </si>
 </sst>
 </file>
@@ -408,7 +414,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -422,7 +428,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B1" s="2">
         <v>3.68</v>
@@ -430,7 +436,7 @@
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2">
         <v>3.68</v>
@@ -454,7 +460,7 @@
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2">
         <v>2.9550000000000001</v>
@@ -462,18 +468,34 @@
     </row>
     <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" s="5">
-        <v>71220</v>
+        <v>45500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2.68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2.68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>